<commit_message>
Add items, vendor names
</commit_message>
<xml_diff>
--- a/data/materials.xlsx
+++ b/data/materials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hi\Store\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CADD8DA9-E8B1-4798-8571-C1968C97E07C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{707E09D0-E454-4BD9-B0D9-C6A666674AB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="308">
   <si>
     <t>Item</t>
   </si>
@@ -919,6 +919,45 @@
   </si>
   <si>
     <t>Maintainance &amp; Repair</t>
+  </si>
+  <si>
+    <t>HRT Roll(Tissue roll)</t>
+  </si>
+  <si>
+    <t>Banana</t>
+  </si>
+  <si>
+    <t>Electric Material</t>
+  </si>
+  <si>
+    <t>Plumbing Material</t>
+  </si>
+  <si>
+    <t>Hardware material</t>
+  </si>
+  <si>
+    <t>Kitchenware</t>
+  </si>
+  <si>
+    <t>CP Pomegranate</t>
+  </si>
+  <si>
+    <t>CP Watermelone</t>
+  </si>
+  <si>
+    <t>CP Pineapple</t>
+  </si>
+  <si>
+    <t>CP Blackcane</t>
+  </si>
+  <si>
+    <t>CP Classic Cane</t>
+  </si>
+  <si>
+    <t>CP ABC</t>
+  </si>
+  <si>
+    <t>Incense Stick (Agarbatthi)</t>
   </si>
 </sst>
 </file>
@@ -1036,7 +1075,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
@@ -1070,6 +1109,7 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1559,13 +1599,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A295"/>
+  <dimension ref="A1:A308"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B276" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B300" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2:A295"/>
+      <selection pane="bottomRight" activeCell="A308" sqref="A308"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -3048,6 +3088,71 @@
         <v>294</v>
       </c>
     </row>
+    <row r="296" spans="1:1">
+      <c r="A296" s="14" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="297" spans="1:1">
+      <c r="A297" s="14" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="298" spans="1:1">
+      <c r="A298" s="14" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="299" spans="1:1">
+      <c r="A299" s="14" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="300" spans="1:1">
+      <c r="A300" s="14" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="301" spans="1:1">
+      <c r="A301" s="14" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="302" spans="1:1">
+      <c r="A302" s="14" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="303" spans="1:1">
+      <c r="A303" s="14" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="304" spans="1:1">
+      <c r="A304" s="14" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="305" spans="1:1">
+      <c r="A305" s="14" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="306" spans="1:1">
+      <c r="A306" s="14" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="307" spans="1:1">
+      <c r="A307" s="14" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="308" spans="1:1">
+      <c r="A308" s="14" t="s">
+        <v>307</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="0.39305555555555599" bottom="0.156944444444444" header="0.23611111111111099" footer="7.8472222222222193E-2"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added items in sheet
</commit_message>
<xml_diff>
--- a/data/materials.xlsx
+++ b/data/materials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hi\Store\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{707E09D0-E454-4BD9-B0D9-C6A666674AB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA3135EF-B04E-4ABA-B714-5A5F957B60F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="314">
   <si>
     <t>Item</t>
   </si>
@@ -958,6 +958,24 @@
   </si>
   <si>
     <t>Incense Stick (Agarbatthi)</t>
+  </si>
+  <si>
+    <t>Coffee_brass_set</t>
+  </si>
+  <si>
+    <t>Ulavacharu</t>
+  </si>
+  <si>
+    <t>Milk_bread</t>
+  </si>
+  <si>
+    <t>pen</t>
+  </si>
+  <si>
+    <t>battery</t>
+  </si>
+  <si>
+    <t>silver_pouch</t>
   </si>
 </sst>
 </file>
@@ -1599,13 +1617,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A308"/>
+  <dimension ref="A1:A314"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B300" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B297" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A308" sqref="A308"/>
+      <selection pane="bottomRight" activeCell="A315" sqref="A315"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -3089,68 +3107,98 @@
       </c>
     </row>
     <row r="296" spans="1:1">
-      <c r="A296" s="14" t="s">
+      <c r="A296" s="13" t="s">
         <v>295</v>
       </c>
     </row>
     <row r="297" spans="1:1">
-      <c r="A297" s="14" t="s">
+      <c r="A297" s="13" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="298" spans="1:1">
-      <c r="A298" s="14" t="s">
+      <c r="A298" s="13" t="s">
         <v>297</v>
       </c>
     </row>
     <row r="299" spans="1:1">
-      <c r="A299" s="14" t="s">
+      <c r="A299" s="13" t="s">
         <v>298</v>
       </c>
     </row>
     <row r="300" spans="1:1">
-      <c r="A300" s="14" t="s">
+      <c r="A300" s="13" t="s">
         <v>299</v>
       </c>
     </row>
     <row r="301" spans="1:1">
-      <c r="A301" s="14" t="s">
+      <c r="A301" s="13" t="s">
         <v>300</v>
       </c>
     </row>
     <row r="302" spans="1:1">
-      <c r="A302" s="14" t="s">
+      <c r="A302" s="13" t="s">
         <v>301</v>
       </c>
     </row>
     <row r="303" spans="1:1">
-      <c r="A303" s="14" t="s">
+      <c r="A303" s="13" t="s">
         <v>302</v>
       </c>
     </row>
     <row r="304" spans="1:1">
-      <c r="A304" s="14" t="s">
+      <c r="A304" s="13" t="s">
         <v>303</v>
       </c>
     </row>
     <row r="305" spans="1:1">
-      <c r="A305" s="14" t="s">
+      <c r="A305" s="13" t="s">
         <v>304</v>
       </c>
     </row>
     <row r="306" spans="1:1">
-      <c r="A306" s="14" t="s">
+      <c r="A306" s="13" t="s">
         <v>305</v>
       </c>
     </row>
     <row r="307" spans="1:1">
-      <c r="A307" s="14" t="s">
+      <c r="A307" s="13" t="s">
         <v>306</v>
       </c>
     </row>
     <row r="308" spans="1:1">
-      <c r="A308" s="14" t="s">
+      <c r="A308" s="13" t="s">
         <v>307</v>
+      </c>
+    </row>
+    <row r="309" spans="1:1">
+      <c r="A309" s="14" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="310" spans="1:1">
+      <c r="A310" s="14" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="311" spans="1:1">
+      <c r="A311" s="14" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="312" spans="1:1">
+      <c r="A312" s="14" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="313" spans="1:1">
+      <c r="A313" s="14" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="314" spans="1:1">
+      <c r="A314" s="14" t="s">
+        <v>313</v>
       </c>
     </row>
   </sheetData>

</xml_diff>